<commit_message>
added row column and removed delete and edit features
</commit_message>
<xml_diff>
--- a/public/bulk_upload_template.xlsx
+++ b/public/bulk_upload_template.xlsx
@@ -31,16 +31,10 @@
     <style:style style:name="co1" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="0.5811in"/>
     </style:style>
-    <style:style style:name="co2" style:family="table-column">
-      <style:table-column-properties fo:break-before="auto" style:column-width="0.7937in"/>
-    </style:style>
     <style:style style:name="ro1" style:family="table-row">
       <style:table-row-properties style:row-height="0.1953in" fo:break-before="auto" style:use-optimal-row-height="true"/>
     </style:style>
-    <style:style style:name="ta1" style:family="table" style:master-page-name="PageStyle_5f_Jobs">
-      <style:table-properties table:display="true" style:writing-mode="lr-tb"/>
-    </style:style>
-    <style:style style:name="ta2" style:family="table" style:master-page-name="PageStyle_5f_user">
+    <style:style style:name="ta1" style:family="table" style:master-page-name="PageStyle_5f_user">
       <style:table-properties table:display="true" style:writing-mode="lr-tb"/>
     </style:style>
   </office:automatic-styles>
@@ -49,55 +43,10 @@
       <table:calculation-settings table:case-sensitive="false" table:automatic-find-labels="false" table:use-regular-expressions="false">
         <table:iteration table:maximum-difference="0.0001"/>
       </table:calculation-settings>
-      <table:table table:name="Jobs" table:style-name="ta1" table:print="false">
-        <office:forms form:automatic-focus="false" form:apply-design-mode="false"/>
-        <table:table-column table:style-name="co1" table:number-columns-repeated="4" table:default-cell-style-name="Excel_20_Built-in_20_Normal"/>
-        <table:table-column table:style-name="co2" table:default-cell-style-name="Excel_20_Built-in_20_Normal"/>
-        <table:table-column table:style-name="co1" table:number-columns-repeated="1019" table:default-cell-style-name="Excel_20_Built-in_20_Normal"/>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string">
-            <text:p>job_id</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string">
-            <text:p>job_name</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string">
-            <text:p>job_desc</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string">
-            <text:p>job_time</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string">
-            <text:p>immediate</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string">
-            <text:p>rerun</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string">
-            <text:p>phone_call</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string">
-            <text:p>email</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string">
-            <text:p>whatsapp</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1015"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1" table:number-rows-repeated="1048574">
-          <table:table-cell table:number-columns-repeated="1024"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell table:number-columns-repeated="1024"/>
-        </table:table-row>
-      </table:table>
-      <table:table table:name="user" table:style-name="ta2" table:print="false">
+      <table:table table:name="user" table:style-name="ta1" table:print="false">
         <office:forms form:automatic-focus="false" form:apply-design-mode="false"/>
         <table:table-column table:style-name="co1" table:number-columns-repeated="1024" table:default-cell-style-name="Excel_20_Built-in_20_Normal"/>
         <table:table-row table:style-name="ro1">
-          <table:table-cell table:style-name="Default" office:value-type="string">
-            <text:p>Job_Id</text:p>
-          </table:table-cell>
           <table:table-cell office:value-type="string">
             <text:p>Name</text:p>
           </table:table-cell>
@@ -107,6 +56,7 @@
           <table:table-cell office:value-type="string">
             <text:p>Phone</text:p>
           </table:table-cell>
+          <table:table-cell table:style-name="Default"/>
           <table:table-cell table:number-columns-repeated="1020"/>
         </table:table-row>
         <table:table-row table:style-name="ro1" table:number-rows-repeated="1048574">
@@ -124,10 +74,12 @@
 <file path=meta.xml><?xml version="1.0" encoding="utf-8"?>
 <office:document-meta xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:grddl="http://www.w3.org/2003/g/data-view#" office:version="1.2">
   <office:meta>
-    <dc:date>2024-05-27T12:57:32.03</dc:date>
+    <dc:date>2024-05-30T12:56:54.01</dc:date>
     <dc:creator>Animesh Anand</dc:creator>
-    <meta:document-statistic meta:table-count="2" meta:cell-count="13" meta:object-count="0"/>
     <meta:generator>OpenOffice/4.1.15$Win32 OpenOffice.org_project/4115m2$Build-9813</meta:generator>
+    <meta:editing-duration>PT37S</meta:editing-duration>
+    <meta:editing-cycles>1</meta:editing-cycles>
+    <meta:document-statistic meta:table-count="1" meta:cell-count="3" meta:object-count="0"/>
   </office:meta>
 </office:document-meta>
 </file>
@@ -138,31 +90,15 @@
     <config:config-item-set config:name="ooo:view-settings">
       <config:config-item config:name="VisibleAreaTop" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaLeft" config:type="int">0</config:config-item>
-      <config:config-item config:name="VisibleAreaWidth" config:type="int">13775</config:config-item>
+      <config:config-item config:name="VisibleAreaWidth" config:type="int">4412</config:config-item>
       <config:config-item config:name="VisibleAreaHeight" config:type="int">493</config:config-item>
       <config:config-item-map-indexed config:name="Views">
         <config:config-item-map-entry>
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
           <config:config-item-map-named config:name="Tables">
-            <config:config-item-map-entry config:name="Jobs">
-              <config:config-item config:name="CursorPositionX" config:type="int">0</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">2</config:config-item>
-              <config:config-item config:name="HorizontalSplitMode" config:type="short">0</config:config-item>
-              <config:config-item config:name="VerticalSplitMode" config:type="short">0</config:config-item>
-              <config:config-item config:name="HorizontalSplitPosition" config:type="int">0</config:config-item>
-              <config:config-item config:name="VerticalSplitPosition" config:type="int">0</config:config-item>
-              <config:config-item config:name="ActiveSplitRange" config:type="short">2</config:config-item>
-              <config:config-item config:name="PositionLeft" config:type="int">0</config:config-item>
-              <config:config-item config:name="PositionRight" config:type="int">0</config:config-item>
-              <config:config-item config:name="PositionTop" config:type="int">0</config:config-item>
-              <config:config-item config:name="PositionBottom" config:type="int">0</config:config-item>
-              <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
-              <config:config-item config:name="ZoomValue" config:type="int">100</config:config-item>
-              <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
-            </config:config-item-map-entry>
             <config:config-item-map-entry config:name="user">
-              <config:config-item config:name="CursorPositionX" config:type="int">2</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">4</config:config-item>
+              <config:config-item config:name="CursorPositionX" config:type="int">3</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">5</config:config-item>
               <config:config-item config:name="HorizontalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="VerticalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="HorizontalSplitPosition" config:type="int">0</config:config-item>
@@ -252,103 +188,100 @@
     <number:number-style style:name="N0">
       <number:number number:min-integer-digits="1"/>
     </number:number-style>
+    <number:currency-style style:name="N104P0" style:volatile="true">
+      <number:currency-symbol number:language="en" number:country="US">$</number:currency-symbol>
+      <number:number number:decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+    </number:currency-style>
+    <number:currency-style style:name="N104">
+      <style:text-properties fo:color="#ff0000"/>
+      <number:text>-</number:text>
+      <number:currency-symbol number:language="en" number:country="US">$</number:currency-symbol>
+      <number:number number:decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N104P0"/>
+    </number:currency-style>
     <number:number-style style:name="N8000" number:language="en" number:country="US">
       <number:number number:min-integer-digits="1"/>
     </number:number-style>
-    <number:currency-style style:name="N8116P0" style:volatile="true" number:language="en" number:country="US">
-      <number:currency-symbol/>
-      <number:number number:decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N8116" number:language="en" number:country="US">
-      <number:text>(</number:text>
-      <number:currency-symbol/>
-      <number:number number:decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N8116P0"/>
-    </number:currency-style>
     <number:currency-style style:name="N8117P0" style:volatile="true" number:language="en" number:country="US">
       <number:currency-symbol/>
       <number:number number:decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
       <number:text> </number:text>
     </number:currency-style>
     <number:currency-style style:name="N8117" number:language="en" number:country="US">
+      <number:text>(</number:text>
+      <number:currency-symbol/>
+      <number:number number:decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N8117P0"/>
+    </number:currency-style>
+    <number:currency-style style:name="N8118P0" style:volatile="true" number:language="en" number:country="US">
+      <number:currency-symbol/>
+      <number:number number:decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N8118" number:language="en" number:country="US">
       <style:text-properties fo:color="#ff0000"/>
       <number:text>(</number:text>
       <number:currency-symbol/>
       <number:number number:decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N8117P0"/>
-    </number:currency-style>
-    <number:currency-style style:name="N8118P0" style:volatile="true" number:language="en" number:country="US">
-      <number:currency-symbol/>
-      <number:number number:decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N8118" number:language="en" number:country="US">
-      <number:text>(</number:text>
-      <number:currency-symbol/>
-      <number:number number:decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
       <style:map style:condition="value()&gt;=0" style:apply-style-name="N8118P0"/>
     </number:currency-style>
-    <number:currency-style style:name="N8119P0" style:volatile="true" number:language="en" number:country="US">
-      <number:currency-symbol/>
-      <number:number number:decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N8119" number:language="en" number:country="US">
+    <number:currency-style style:name="N8120P0" style:volatile="true" number:language="en" number:country="US">
+      <number:currency-symbol/>
+      <number:number number:decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N8120" number:language="en" number:country="US">
+      <number:text>(</number:text>
+      <number:currency-symbol/>
+      <number:number number:decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N8120P0"/>
+    </number:currency-style>
+    <number:currency-style style:name="N8121P0" style:volatile="true" number:language="en" number:country="US">
+      <number:currency-symbol/>
+      <number:number number:decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N8121" number:language="en" number:country="US">
       <style:text-properties fo:color="#ff0000"/>
       <number:text>(</number:text>
       <number:currency-symbol/>
       <number:number number:decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N8119P0"/>
-    </number:currency-style>
-    <number:date-style style:name="N8120" number:language="en" number:country="US">
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N8121P0"/>
+    </number:currency-style>
+    <number:date-style style:name="N8122" number:language="en" number:country="US">
       <number:month/>
       <number:text>/</number:text>
       <number:day/>
       <number:text>/</number:text>
       <number:year number:style="long"/>
     </number:date-style>
-    <number:date-style style:name="N8121" number:language="en" number:country="US">
+    <number:date-style style:name="N8123" number:language="en" number:country="US">
       <number:day/>
       <number:text>-</number:text>
       <number:month number:textual="true"/>
       <number:text>-</number:text>
       <number:year/>
     </number:date-style>
-    <number:date-style style:name="N8122" number:language="en" number:country="US">
+    <number:date-style style:name="N8124" number:language="en" number:country="US">
       <number:day/>
       <number:text>-</number:text>
       <number:month number:textual="true"/>
     </number:date-style>
-    <number:date-style style:name="N8123" number:language="en" number:country="US">
+    <number:date-style style:name="N8125" number:language="en" number:country="US">
       <number:month number:textual="true"/>
       <number:text>-</number:text>
       <number:year/>
     </number:date-style>
-    <number:time-style style:name="N8124" number:language="en" number:country="US">
-      <number:hours/>
-      <number:text>:</number:text>
-      <number:minutes number:style="long"/>
-      <number:text> </number:text>
-      <number:am-pm/>
-    </number:time-style>
-    <number:time-style style:name="N8125" number:language="en" number:country="US">
-      <number:hours/>
-      <number:text>:</number:text>
-      <number:minutes number:style="long"/>
-      <number:text>:</number:text>
-      <number:seconds number:style="long"/>
-      <number:text> </number:text>
-      <number:am-pm/>
-    </number:time-style>
     <number:time-style style:name="N8126" number:language="en" number:country="US">
       <number:hours/>
       <number:text>:</number:text>
       <number:minutes number:style="long"/>
+      <number:text> </number:text>
+      <number:am-pm/>
     </number:time-style>
     <number:time-style style:name="N8127" number:language="en" number:country="US">
       <number:hours/>
@@ -356,8 +289,22 @@
       <number:minutes number:style="long"/>
       <number:text>:</number:text>
       <number:seconds number:style="long"/>
-    </number:time-style>
-    <number:date-style style:name="N8128" number:language="en" number:country="US">
+      <number:text> </number:text>
+      <number:am-pm/>
+    </number:time-style>
+    <number:time-style style:name="N8128" number:language="en" number:country="US">
+      <number:hours/>
+      <number:text>:</number:text>
+      <number:minutes number:style="long"/>
+    </number:time-style>
+    <number:time-style style:name="N8129" number:language="en" number:country="US">
+      <number:hours/>
+      <number:text>:</number:text>
+      <number:minutes number:style="long"/>
+      <number:text>:</number:text>
+      <number:seconds number:style="long"/>
+    </number:time-style>
+    <number:date-style style:name="N8130" number:language="en" number:country="US">
       <number:month/>
       <number:text>/</number:text>
       <number:day/>
@@ -368,164 +315,152 @@
       <number:text>:</number:text>
       <number:minutes number:style="long"/>
     </number:date-style>
-    <number:number-style style:name="N8129P0" style:volatile="true" number:language="en" number:country="US">
-      <number:number number:decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:number-style>
-    <number:number-style style:name="N8129" number:language="en" number:country="US">
-      <number:text>(</number:text>
-      <number:number number:decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N8129P0"/>
-    </number:number-style>
-    <number:number-style style:name="N8130P0" style:volatile="true" number:language="en" number:country="US">
-      <number:number number:decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:number-style>
-    <number:number-style style:name="N8130" number:language="en" number:country="US">
+    <number:number-style style:name="N8132P0" style:volatile="true" number:language="en" number:country="US">
+      <number:number number:decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:number-style>
+    <number:number-style style:name="N8132" number:language="en" number:country="US">
+      <number:text>(</number:text>
+      <number:number number:decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N8132P0"/>
+    </number:number-style>
+    <number:number-style style:name="N8133P0" style:volatile="true" number:language="en" number:country="US">
+      <number:number number:decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:number-style>
+    <number:number-style style:name="N8133" number:language="en" number:country="US">
       <style:text-properties fo:color="#ff0000"/>
       <number:text>(</number:text>
       <number:number number:decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N8130P0"/>
-    </number:number-style>
-    <number:number-style style:name="N8131P0" style:volatile="true" number:language="en" number:country="US">
-      <number:number number:decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:number-style>
-    <number:number-style style:name="N8131" number:language="en" number:country="US">
-      <number:text>(</number:text>
-      <number:number number:decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N8131P0"/>
-    </number:number-style>
-    <number:number-style style:name="N8132P0" style:volatile="true" number:language="en" number:country="US">
-      <number:number number:decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:number-style>
-    <number:number-style style:name="N8132" number:language="en" number:country="US">
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N8133P0"/>
+    </number:number-style>
+    <number:number-style style:name="N8135P0" style:volatile="true" number:language="en" number:country="US">
+      <number:number number:decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:number-style>
+    <number:number-style style:name="N8135" number:language="en" number:country="US">
+      <number:text>(</number:text>
+      <number:number number:decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N8135P0"/>
+    </number:number-style>
+    <number:number-style style:name="N8136P0" style:volatile="true" number:language="en" number:country="US">
+      <number:number number:decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:number-style>
+    <number:number-style style:name="N8136" number:language="en" number:country="US">
       <style:text-properties fo:color="#ff0000"/>
       <number:text>(</number:text>
       <number:number number:decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N8132P0"/>
-    </number:number-style>
-    <number:number-style style:name="N8133P0" style:volatile="true" number:language="en" number:country="US">
-      <number:text> </number:text>
-      <number:number number:decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:number-style>
-    <number:number-style style:name="N8133P1" style:volatile="true" number:language="en" number:country="US">
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N8136P0"/>
+    </number:number-style>
+    <number:number-style style:name="N8139P0" style:volatile="true" number:language="en" number:country="US">
+      <number:number number:decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:number-style>
+    <number:number-style style:name="N8139P1" style:volatile="true" number:language="en" number:country="US">
       <number:text> (</number:text>
       <number:number number:decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
     </number:number-style>
-    <number:number-style style:name="N8133P2" style:volatile="true" number:language="en" number:country="US">
+    <number:number-style style:name="N8139P2" style:volatile="true" number:language="en" number:country="US">
       <number:text> - </number:text>
     </number:number-style>
-    <number:text-style style:name="N8133" number:language="en" number:country="US">
-      <number:text> </number:text>
+    <number:text-style style:name="N8139" number:language="en" number:country="US">
       <number:text-content/>
       <number:text> </number:text>
-      <style:map style:condition="value()&gt;0" style:apply-style-name="N8133P0"/>
-      <style:map style:condition="value()&lt;0" style:apply-style-name="N8133P1"/>
-      <style:map style:condition="value()=0" style:apply-style-name="N8133P2"/>
+      <style:map style:condition="value()&gt;0" style:apply-style-name="N8139P0"/>
+      <style:map style:condition="value()&lt;0" style:apply-style-name="N8139P1"/>
+      <style:map style:condition="value()=0" style:apply-style-name="N8139P2"/>
     </number:text-style>
-    <number:currency-style style:name="N8134P0" style:volatile="true" number:language="en" number:country="US">
-      <number:text> </number:text>
-      <number:currency-symbol/>
-      <number:number number:decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N8134P1" style:volatile="true" number:language="en" number:country="US">
-      <number:text> </number:text>
-      <number:currency-symbol/>
-      <number:text>(</number:text>
-      <number:number number:decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N8134P2" style:volatile="true" number:language="en" number:country="US">
-      <number:text> </number:text>
+    <number:currency-style style:name="N8142P0" style:volatile="true" number:language="en" number:country="US">
+      <number:currency-symbol/>
+      <number:number number:decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N8142P1" style:volatile="true" number:language="en" number:country="US">
+      <number:currency-symbol/>
+      <number:text>(</number:text>
+      <number:number number:decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N8142P2" style:volatile="true" number:language="en" number:country="US">
       <number:currency-symbol/>
       <number:text>- </number:text>
     </number:currency-style>
-    <number:text-style style:name="N8134" number:language="en" number:country="US">
-      <number:text> </number:text>
+    <number:text-style style:name="N8142" number:language="en" number:country="US">
       <number:text-content/>
       <number:text> </number:text>
-      <style:map style:condition="value()&gt;0" style:apply-style-name="N8134P0"/>
-      <style:map style:condition="value()&lt;0" style:apply-style-name="N8134P1"/>
-      <style:map style:condition="value()=0" style:apply-style-name="N8134P2"/>
+      <style:map style:condition="value()&gt;0" style:apply-style-name="N8142P0"/>
+      <style:map style:condition="value()&lt;0" style:apply-style-name="N8142P1"/>
+      <style:map style:condition="value()=0" style:apply-style-name="N8142P2"/>
     </number:text-style>
-    <number:number-style style:name="N8135P0" style:volatile="true" number:language="en" number:country="US">
-      <number:text> </number:text>
-      <number:number number:decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:number-style>
-    <number:number-style style:name="N8135P1" style:volatile="true" number:language="en" number:country="US">
+    <number:number-style style:name="N8145P0" style:volatile="true" number:language="en" number:country="US">
+      <number:number number:decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:number-style>
+    <number:number-style style:name="N8145P1" style:volatile="true" number:language="en" number:country="US">
       <number:text> (</number:text>
       <number:number number:decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text>)</number:text>
     </number:number-style>
-    <number:number-style style:name="N8135P2" style:volatile="true" number:language="en" number:country="US">
+    <number:number-style style:name="N8145P2" style:volatile="true" number:language="en" number:country="US">
       <number:text> -</number:text>
       <number:number number:decimal-places="0" number:min-integer-digits="0"/>
       <number:text> </number:text>
     </number:number-style>
-    <number:text-style style:name="N8135" number:language="en" number:country="US">
-      <number:text> </number:text>
+    <number:text-style style:name="N8145" number:language="en" number:country="US">
       <number:text-content/>
       <number:text> </number:text>
-      <style:map style:condition="value()&gt;0" style:apply-style-name="N8135P0"/>
-      <style:map style:condition="value()&lt;0" style:apply-style-name="N8135P1"/>
-      <style:map style:condition="value()=0" style:apply-style-name="N8135P2"/>
+      <style:map style:condition="value()&gt;0" style:apply-style-name="N8145P0"/>
+      <style:map style:condition="value()&lt;0" style:apply-style-name="N8145P1"/>
+      <style:map style:condition="value()=0" style:apply-style-name="N8145P2"/>
     </number:text-style>
-    <number:currency-style style:name="N8136P0" style:volatile="true" number:language="en" number:country="US">
-      <number:text> </number:text>
-      <number:currency-symbol/>
-      <number:number number:decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N8136P1" style:volatile="true" number:language="en" number:country="US">
-      <number:text> </number:text>
-      <number:currency-symbol/>
-      <number:text>(</number:text>
-      <number:number number:decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text>)</number:text>
-    </number:currency-style>
-    <number:currency-style style:name="N8136P2" style:volatile="true" number:language="en" number:country="US">
-      <number:text> </number:text>
+    <number:currency-style style:name="N8148P0" style:volatile="true" number:language="en" number:country="US">
+      <number:currency-symbol/>
+      <number:number number:decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N8148P1" style:volatile="true" number:language="en" number:country="US">
+      <number:currency-symbol/>
+      <number:text>(</number:text>
+      <number:number number:decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text>)</number:text>
+    </number:currency-style>
+    <number:currency-style style:name="N8148P2" style:volatile="true" number:language="en" number:country="US">
       <number:currency-symbol/>
       <number:text>-</number:text>
       <number:number number:decimal-places="0" number:min-integer-digits="0"/>
       <number:text> </number:text>
     </number:currency-style>
-    <number:text-style style:name="N8136" number:language="en" number:country="US">
-      <number:text> </number:text>
+    <number:text-style style:name="N8148" number:language="en" number:country="US">
       <number:text-content/>
       <number:text> </number:text>
-      <style:map style:condition="value()&gt;0" style:apply-style-name="N8136P0"/>
-      <style:map style:condition="value()&lt;0" style:apply-style-name="N8136P1"/>
-      <style:map style:condition="value()=0" style:apply-style-name="N8136P2"/>
+      <style:map style:condition="value()&gt;0" style:apply-style-name="N8148P0"/>
+      <style:map style:condition="value()&lt;0" style:apply-style-name="N8148P1"/>
+      <style:map style:condition="value()=0" style:apply-style-name="N8148P2"/>
     </number:text-style>
-    <number:time-style style:name="N8137" number:language="en" number:country="US">
+    <number:time-style style:name="N8149" number:language="en" number:country="US">
       <number:minutes number:style="long"/>
       <number:text>:</number:text>
       <number:seconds number:style="long"/>
     </number:time-style>
-    <number:time-style style:name="N8138" number:language="en" number:country="US" number:truncate-on-overflow="false">
+    <number:time-style style:name="N8150" number:language="en" number:country="US" number:truncate-on-overflow="false">
       <number:hours/>
       <number:text>:</number:text>
       <number:minutes number:style="long"/>
       <number:text>:</number:text>
       <number:seconds number:style="long"/>
     </number:time-style>
-    <number:time-style style:name="N8139" number:language="en" number:country="US">
+    <number:time-style style:name="N8151" number:language="en" number:country="US">
       <number:minutes number:style="long"/>
       <number:text>:</number:text>
       <number:seconds number:style="long" number:decimal-places="1"/>
     </number:time-style>
-    <number:number-style style:name="N8140" number:language="en" number:country="US">
+    <number:number-style style:name="N8152" number:language="en" number:country="US">
       <number:scientific-number number:decimal-places="1" number:min-integer-digits="3" number:min-exponent-digits="1"/>
     </number:number-style>
     <style:style style:name="Default" style:family="table-cell">
@@ -534,7 +469,7 @@
     <style:style style:name="Result" style:family="table-cell" style:parent-style-name="Default">
       <style:text-properties fo:font-style="italic" style:text-underline-style="solid" style:text-underline-width="auto" style:text-underline-color="font-color" fo:font-weight="bold"/>
     </style:style>
-    <style:style style:name="Result2" style:family="table-cell" style:parent-style-name="Result"/>
+    <style:style style:name="Result2" style:family="table-cell" style:parent-style-name="Result" style:data-style-name="N104"/>
     <style:style style:name="Heading" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties style:text-align-source="fix" style:repeat-content="false"/>
       <style:paragraph-properties fo:text-align="center"/>
@@ -610,9 +545,9 @@
         </style:region-left>
         <style:region-right>
           <text:p>
-            <text:date style:data-style-name="N2" text:date-value="2024-05-27">05/27/2024</text:date>
+            <text:date style:data-style-name="N2" text:date-value="2024-05-30">05/30/2024</text:date>
             , 
-            <text:time>12:57:32</text:time>
+            <text:time>12:56:54</text:time>
           </text:p>
         </style:region-right>
       </style:header>

</xml_diff>